<commit_message>
Added Q dG sensitivity analysis
</commit_message>
<xml_diff>
--- a/Matt_Matlab/Data Compilation for Paper/Supplementary_Materials_09_11.xlsx
+++ b/Matt_Matlab/Data Compilation for Paper/Supplementary_Materials_09_11.xlsx
@@ -17547,7 +17547,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -17557,6 +17557,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -17588,7 +17594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -17635,6 +17641,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -19369,13 +19384,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M707"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="A689" workbookViewId="0">
+      <selection activeCell="E720" sqref="E720"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" style="4" customWidth="1"/>
     <col min="2" max="7" width="9.140625" style="4"/>
     <col min="8" max="10" width="9.140625" style="15"/>
     <col min="11" max="11" width="15.85546875" style="15" bestFit="1" customWidth="1"/>
@@ -33350,36 +33365,36 @@
       <c r="L376" s="14"/>
       <c r="M376" s="14"/>
     </row>
-    <row r="377" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A377" s="3" t="s">
+    <row r="377" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A377" s="20" t="s">
         <v>1961</v>
       </c>
-      <c r="B377" s="3" t="s">
+      <c r="B377" s="20" t="s">
         <v>1962</v>
       </c>
-      <c r="C377" s="3"/>
-      <c r="D377" s="3" t="s">
+      <c r="C377" s="20"/>
+      <c r="D377" s="20" t="s">
         <v>1963</v>
       </c>
-      <c r="E377" s="3"/>
-      <c r="F377" s="3"/>
-      <c r="G377" s="3" t="s">
+      <c r="E377" s="20"/>
+      <c r="F377" s="20"/>
+      <c r="G377" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H377" s="14">
-        <v>0</v>
-      </c>
-      <c r="I377" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J377" s="14">
-        <v>0</v>
-      </c>
-      <c r="K377" s="14" t="s">
+      <c r="H377" s="21">
+        <v>0</v>
+      </c>
+      <c r="I377" s="21">
+        <v>1000</v>
+      </c>
+      <c r="J377" s="21">
+        <v>0</v>
+      </c>
+      <c r="K377" s="21" t="s">
         <v>1160</v>
       </c>
-      <c r="L377" s="14"/>
-      <c r="M377" s="14"/>
+      <c r="L377" s="21"/>
+      <c r="M377" s="21"/>
     </row>
     <row r="378" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A378" s="3" t="s">
@@ -33453,36 +33468,36 @@
       <c r="L379" s="14"/>
       <c r="M379" s="14"/>
     </row>
-    <row r="380" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A380" s="3" t="s">
+    <row r="380" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A380" s="20" t="s">
         <v>1973</v>
       </c>
-      <c r="B380" s="3" t="s">
+      <c r="B380" s="20" t="s">
         <v>1974</v>
       </c>
-      <c r="C380" s="3"/>
-      <c r="D380" s="3" t="s">
+      <c r="C380" s="20"/>
+      <c r="D380" s="20" t="s">
         <v>1975</v>
       </c>
-      <c r="E380" s="3"/>
-      <c r="F380" s="3"/>
-      <c r="G380" s="3" t="s">
+      <c r="E380" s="20"/>
+      <c r="F380" s="20"/>
+      <c r="G380" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H380" s="14">
-        <v>0</v>
-      </c>
-      <c r="I380" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J380" s="14">
-        <v>0</v>
-      </c>
-      <c r="K380" s="14" t="s">
+      <c r="H380" s="21">
+        <v>0</v>
+      </c>
+      <c r="I380" s="21">
+        <v>1000</v>
+      </c>
+      <c r="J380" s="21">
+        <v>0</v>
+      </c>
+      <c r="K380" s="21" t="s">
         <v>1160</v>
       </c>
-      <c r="L380" s="14"/>
-      <c r="M380" s="14"/>
+      <c r="L380" s="21"/>
+      <c r="M380" s="21"/>
     </row>
     <row r="381" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A381" s="3" t="s">
@@ -34363,36 +34378,36 @@
       <c r="L405" s="14"/>
       <c r="M405" s="14"/>
     </row>
-    <row r="406" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A406" s="3" t="s">
+    <row r="406" spans="1:13" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A406" s="20" t="s">
         <v>2095</v>
       </c>
-      <c r="B406" s="3" t="s">
+      <c r="B406" s="20" t="s">
         <v>2096</v>
       </c>
-      <c r="C406" s="3"/>
-      <c r="D406" s="3" t="s">
+      <c r="C406" s="20"/>
+      <c r="D406" s="20" t="s">
         <v>2097</v>
       </c>
-      <c r="E406" s="3"/>
-      <c r="F406" s="3"/>
-      <c r="G406" s="3" t="s">
+      <c r="E406" s="20"/>
+      <c r="F406" s="20"/>
+      <c r="G406" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H406" s="14">
-        <v>0</v>
-      </c>
-      <c r="I406" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J406" s="14">
-        <v>0</v>
-      </c>
-      <c r="K406" s="14" t="s">
+      <c r="H406" s="21">
+        <v>0</v>
+      </c>
+      <c r="I406" s="21">
+        <v>1000</v>
+      </c>
+      <c r="J406" s="21">
+        <v>0</v>
+      </c>
+      <c r="K406" s="21" t="s">
         <v>1160</v>
       </c>
-      <c r="L406" s="14"/>
-      <c r="M406" s="14"/>
+      <c r="L406" s="21"/>
+      <c r="M406" s="21"/>
     </row>
     <row r="407" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A407" s="3" t="s">
@@ -34503,38 +34518,38 @@
       <c r="L409" s="14"/>
       <c r="M409" s="14"/>
     </row>
-    <row r="410" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A410" s="3" t="s">
+    <row r="410" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A410" s="20" t="s">
         <v>2116</v>
       </c>
-      <c r="B410" s="3" t="s">
+      <c r="B410" s="20" t="s">
         <v>2117</v>
       </c>
-      <c r="C410" s="3"/>
-      <c r="D410" s="3" t="s">
+      <c r="C410" s="20"/>
+      <c r="D410" s="20" t="s">
         <v>2118</v>
       </c>
-      <c r="E410" s="3" t="s">
+      <c r="E410" s="20" t="s">
         <v>2119</v>
       </c>
-      <c r="F410" s="3"/>
-      <c r="G410" s="3" t="s">
+      <c r="F410" s="20"/>
+      <c r="G410" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H410" s="14">
-        <v>0</v>
-      </c>
-      <c r="I410" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J410" s="14">
-        <v>0</v>
-      </c>
-      <c r="K410" s="14" t="s">
+      <c r="H410" s="21">
+        <v>0</v>
+      </c>
+      <c r="I410" s="21">
+        <v>1000</v>
+      </c>
+      <c r="J410" s="21">
+        <v>0</v>
+      </c>
+      <c r="K410" s="21" t="s">
         <v>1160</v>
       </c>
-      <c r="L410" s="14"/>
-      <c r="M410" s="14"/>
+      <c r="L410" s="21"/>
+      <c r="M410" s="21"/>
     </row>
     <row r="411" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A411" s="3" t="s">
@@ -34676,36 +34691,36 @@
       <c r="L414" s="14"/>
       <c r="M414" s="14"/>
     </row>
-    <row r="415" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A415" s="3" t="s">
+    <row r="415" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A415" s="20" t="s">
         <v>2138</v>
       </c>
-      <c r="B415" s="3" t="s">
+      <c r="B415" s="20" t="s">
         <v>2139</v>
       </c>
-      <c r="C415" s="3"/>
-      <c r="D415" s="3" t="s">
+      <c r="C415" s="20"/>
+      <c r="D415" s="20" t="s">
         <v>2140</v>
       </c>
-      <c r="E415" s="3"/>
-      <c r="F415" s="3"/>
-      <c r="G415" s="3" t="s">
+      <c r="E415" s="20"/>
+      <c r="F415" s="20"/>
+      <c r="G415" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H415" s="14">
-        <v>0</v>
-      </c>
-      <c r="I415" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J415" s="14">
-        <v>0</v>
-      </c>
-      <c r="K415" s="14" t="s">
+      <c r="H415" s="21">
+        <v>0</v>
+      </c>
+      <c r="I415" s="21">
+        <v>1000</v>
+      </c>
+      <c r="J415" s="21">
+        <v>0</v>
+      </c>
+      <c r="K415" s="21" t="s">
         <v>1160</v>
       </c>
-      <c r="L415" s="14"/>
-      <c r="M415" s="14"/>
+      <c r="L415" s="21"/>
+      <c r="M415" s="21"/>
     </row>
     <row r="416" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A416" s="3" t="s">
@@ -35219,36 +35234,36 @@
       <c r="L429" s="14"/>
       <c r="M429" s="14"/>
     </row>
-    <row r="430" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A430" s="3" t="s">
+    <row r="430" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A430" s="20" t="s">
         <v>2217</v>
       </c>
-      <c r="B430" s="3" t="s">
+      <c r="B430" s="20" t="s">
         <v>2218</v>
       </c>
-      <c r="C430" s="3"/>
-      <c r="D430" s="3" t="s">
+      <c r="C430" s="20"/>
+      <c r="D430" s="20" t="s">
         <v>2219</v>
       </c>
-      <c r="E430" s="3"/>
-      <c r="F430" s="3"/>
-      <c r="G430" s="3" t="s">
+      <c r="E430" s="20"/>
+      <c r="F430" s="20"/>
+      <c r="G430" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H430" s="14">
-        <v>0</v>
-      </c>
-      <c r="I430" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J430" s="14">
-        <v>0</v>
-      </c>
-      <c r="K430" s="14" t="s">
+      <c r="H430" s="21">
+        <v>0</v>
+      </c>
+      <c r="I430" s="21">
+        <v>1000</v>
+      </c>
+      <c r="J430" s="21">
+        <v>0</v>
+      </c>
+      <c r="K430" s="21" t="s">
         <v>1160</v>
       </c>
-      <c r="L430" s="14"/>
-      <c r="M430" s="14"/>
+      <c r="L430" s="21"/>
+      <c r="M430" s="21"/>
     </row>
     <row r="431" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A431" s="3" t="s">
@@ -35645,36 +35660,36 @@
       <c r="L441" s="14"/>
       <c r="M441" s="14"/>
     </row>
-    <row r="442" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A442" s="3" t="s">
+    <row r="442" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A442" s="20" t="s">
         <v>2275</v>
       </c>
-      <c r="B442" s="3" t="s">
+      <c r="B442" s="20" t="s">
         <v>2276</v>
       </c>
-      <c r="C442" s="3"/>
-      <c r="D442" s="3" t="s">
+      <c r="C442" s="20"/>
+      <c r="D442" s="20" t="s">
         <v>2277</v>
       </c>
-      <c r="E442" s="3"/>
-      <c r="F442" s="3"/>
-      <c r="G442" s="3" t="s">
+      <c r="E442" s="20"/>
+      <c r="F442" s="20"/>
+      <c r="G442" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H442" s="14">
-        <v>0</v>
-      </c>
-      <c r="I442" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J442" s="14">
-        <v>0</v>
-      </c>
-      <c r="K442" s="14" t="s">
+      <c r="H442" s="21">
+        <v>0</v>
+      </c>
+      <c r="I442" s="21">
+        <v>1000</v>
+      </c>
+      <c r="J442" s="21">
+        <v>0</v>
+      </c>
+      <c r="K442" s="21" t="s">
         <v>1160</v>
       </c>
-      <c r="L442" s="14"/>
-      <c r="M442" s="14"/>
+      <c r="L442" s="21"/>
+      <c r="M442" s="21"/>
     </row>
     <row r="443" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A443" s="3" t="s">
@@ -35890,36 +35905,36 @@
       <c r="L448" s="14"/>
       <c r="M448" s="14"/>
     </row>
-    <row r="449" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A449" s="3" t="s">
+    <row r="449" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A449" s="20" t="s">
         <v>2309</v>
       </c>
-      <c r="B449" s="3" t="s">
+      <c r="B449" s="20" t="s">
         <v>2310</v>
       </c>
-      <c r="C449" s="3"/>
-      <c r="D449" s="3" t="s">
+      <c r="C449" s="20"/>
+      <c r="D449" s="20" t="s">
         <v>2311</v>
       </c>
-      <c r="E449" s="3"/>
-      <c r="F449" s="3"/>
-      <c r="G449" s="3" t="s">
+      <c r="E449" s="20"/>
+      <c r="F449" s="20"/>
+      <c r="G449" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H449" s="14">
-        <v>0</v>
-      </c>
-      <c r="I449" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J449" s="14">
-        <v>0</v>
-      </c>
-      <c r="K449" s="14" t="s">
+      <c r="H449" s="21">
+        <v>0</v>
+      </c>
+      <c r="I449" s="21">
+        <v>1000</v>
+      </c>
+      <c r="J449" s="21">
+        <v>0</v>
+      </c>
+      <c r="K449" s="21" t="s">
         <v>1160</v>
       </c>
-      <c r="L449" s="14"/>
-      <c r="M449" s="14"/>
+      <c r="L449" s="21"/>
+      <c r="M449" s="21"/>
     </row>
     <row r="450" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A450" s="3" t="s">
@@ -35997,36 +36012,36 @@
       <c r="L451" s="14"/>
       <c r="M451" s="14"/>
     </row>
-    <row r="452" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A452" s="3" t="s">
+    <row r="452" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A452" s="20" t="s">
         <v>2323</v>
       </c>
-      <c r="B452" s="3" t="s">
+      <c r="B452" s="20" t="s">
         <v>2324</v>
       </c>
-      <c r="C452" s="3"/>
-      <c r="D452" s="3" t="s">
+      <c r="C452" s="20"/>
+      <c r="D452" s="20" t="s">
         <v>2325</v>
       </c>
-      <c r="E452" s="3"/>
-      <c r="F452" s="3"/>
-      <c r="G452" s="3" t="s">
+      <c r="E452" s="20"/>
+      <c r="F452" s="20"/>
+      <c r="G452" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H452" s="14">
-        <v>0</v>
-      </c>
-      <c r="I452" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J452" s="14">
-        <v>0</v>
-      </c>
-      <c r="K452" s="14" t="s">
+      <c r="H452" s="21">
+        <v>0</v>
+      </c>
+      <c r="I452" s="21">
+        <v>1000</v>
+      </c>
+      <c r="J452" s="21">
+        <v>0</v>
+      </c>
+      <c r="K452" s="21" t="s">
         <v>1160</v>
       </c>
-      <c r="L452" s="14"/>
-      <c r="M452" s="14"/>
+      <c r="L452" s="21"/>
+      <c r="M452" s="21"/>
     </row>
     <row r="453" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A453" s="3" t="s">
@@ -36168,36 +36183,36 @@
       <c r="L456" s="14"/>
       <c r="M456" s="14"/>
     </row>
-    <row r="457" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A457" s="3" t="s">
+    <row r="457" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A457" s="20" t="s">
         <v>2346</v>
       </c>
-      <c r="B457" s="3" t="s">
+      <c r="B457" s="20" t="s">
         <v>2347</v>
       </c>
-      <c r="C457" s="3"/>
-      <c r="D457" s="3" t="s">
+      <c r="C457" s="20"/>
+      <c r="D457" s="20" t="s">
         <v>2348</v>
       </c>
-      <c r="E457" s="3"/>
-      <c r="F457" s="3"/>
-      <c r="G457" s="3" t="s">
+      <c r="E457" s="20"/>
+      <c r="F457" s="20"/>
+      <c r="G457" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H457" s="14">
-        <v>0</v>
-      </c>
-      <c r="I457" s="14">
-        <v>1000</v>
-      </c>
-      <c r="J457" s="14">
-        <v>0</v>
-      </c>
-      <c r="K457" s="14" t="s">
+      <c r="H457" s="21">
+        <v>0</v>
+      </c>
+      <c r="I457" s="21">
+        <v>1000</v>
+      </c>
+      <c r="J457" s="21">
+        <v>0</v>
+      </c>
+      <c r="K457" s="21" t="s">
         <v>1160</v>
       </c>
-      <c r="L457" s="14"/>
-      <c r="M457" s="14"/>
+      <c r="L457" s="21"/>
+      <c r="M457" s="21"/>
     </row>
     <row r="458" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A458" s="3" t="s">

</xml_diff>